<commit_message>
update sawsdl script to have documentation
</commit_message>
<xml_diff>
--- a/src/main/scripts/add_sawsdl_references/input_files/Apollo-XSD-to-Classes-mappings.xlsx
+++ b/src/main/scripts/add_sawsdl_references/input_files/Apollo-XSD-to-Classes-mappings.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
-  <workbookPr/>
+  <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amd176/Documents/Repositories/apollo-xsd-and-types/src/main/scripts/add_sawsdl_references/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="460" windowWidth="25600" windowHeight="20020" tabRatio="500"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Apollo Types" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="941">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="943">
   <si>
     <t>Probability</t>
   </si>
@@ -2673,27 +2673,18 @@
     <t>disease transmission model identifier</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/APOLLO_SV00000524</t>
-  </si>
-  <si>
     <t>total disease cases</t>
   </si>
   <si>
     <t>total fatal disease cases</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/APOLLO_SV00000525</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/OMRSE_00000098</t>
   </si>
   <si>
     <t>racial identity datum</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/APOLLO_SV00000523</t>
-  </si>
-  <si>
     <t>employment status data item</t>
   </si>
   <si>
@@ -2838,9 +2829,6 @@
     <t>contaminated abiotic thing</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/APOLLO_SV00000522</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/UO_0000003</t>
   </si>
   <si>
@@ -2851,13 +2839,31 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/UO_0000191</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/APOLLO_SV_00000571</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/APOLLO_SV_00000569</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/APOLLO_SV_00000568</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/APOLLO_SV_00000570</t>
+  </si>
+  <si>
+    <t>apolloLocationCode</t>
+  </si>
+  <si>
+    <t>locationDefinition</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2901,6 +2907,13 @@
       <color rgb="FF000000"/>
       <name val="Arial Unicode MS"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2928,25 +2941,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2955,6 +2973,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -3003,7 +3024,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -3038,7 +3059,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -3225,11 +3246,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C140"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="44" customWidth="1"/>
     <col min="2" max="2" width="42.1640625" style="2" customWidth="1"/>
@@ -3266,7 +3287,7 @@
         <v>194</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>940</v>
+        <v>936</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -4179,7 +4200,7 @@
         <v>466</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>938</v>
+        <v>934</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -4245,7 +4266,7 @@
         <v>471</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
@@ -4673,7 +4694,7 @@
       <c r="B131" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="C131" s="2" t="s">
+      <c r="C131" s="6" t="s">
         <v>663</v>
       </c>
     </row>
@@ -4728,7 +4749,7 @@
       <c r="B136" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="C136" s="2" t="s">
+      <c r="C136" s="6" t="s">
         <v>671</v>
       </c>
     </row>
@@ -4778,19 +4799,19 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D164"/>
+  <dimension ref="A1:D166"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="A168" sqref="A168"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38" customWidth="1"/>
     <col min="2" max="2" width="42.83203125" customWidth="1"/>
@@ -4809,7 +4830,7 @@
         <v>300</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18" thickTop="1" x14ac:dyDescent="0.25">
@@ -4865,7 +4886,7 @@
         <v>675</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -4879,7 +4900,7 @@
         <v>309</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>891</v>
+        <v>888</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -4921,7 +4942,7 @@
         <v>676</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>892</v>
+        <v>889</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -4977,7 +4998,7 @@
         <v>683</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>893</v>
+        <v>890</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -5047,7 +5068,7 @@
         <v>313</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>899</v>
+        <v>896</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -5061,7 +5082,7 @@
         <v>314</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -5075,7 +5096,7 @@
         <v>315</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -5089,7 +5110,7 @@
         <v>690</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -5103,7 +5124,7 @@
         <v>692</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -5117,7 +5138,7 @@
         <v>695</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -5128,10 +5149,10 @@
         <v>696</v>
       </c>
       <c r="C24" t="s">
-        <v>937</v>
+        <v>933</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -5145,7 +5166,7 @@
         <v>697</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -5159,7 +5180,7 @@
         <v>316</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>898</v>
+        <v>895</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -5243,7 +5264,7 @@
         <v>700</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>901</v>
+        <v>898</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -5257,7 +5278,7 @@
         <v>321</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -5271,7 +5292,7 @@
         <v>322</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -5285,7 +5306,7 @@
         <v>323</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -5299,7 +5320,7 @@
         <v>702</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -5397,7 +5418,7 @@
         <v>328</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>903</v>
+        <v>900</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -5439,7 +5460,7 @@
         <v>711</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -5453,7 +5474,7 @@
         <v>712</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -5467,7 +5488,7 @@
         <v>714</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -5523,7 +5544,7 @@
         <v>715</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -5537,7 +5558,7 @@
         <v>332</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -5565,7 +5586,7 @@
         <v>716</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>909</v>
+        <v>906</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -5635,7 +5656,7 @@
         <v>720</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>910</v>
+        <v>907</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -5649,7 +5670,7 @@
         <v>722</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>911</v>
+        <v>908</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -5663,7 +5684,7 @@
         <v>724</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -5677,7 +5698,7 @@
         <v>726</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -5691,7 +5712,7 @@
         <v>728</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -5719,7 +5740,7 @@
         <v>732</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>914</v>
+        <v>911</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -5743,11 +5764,11 @@
       <c r="B68" t="s">
         <v>737</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="6" t="s">
         <v>736</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>915</v>
+        <v>912</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -5761,7 +5782,7 @@
         <v>738</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>916</v>
+        <v>913</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -5831,7 +5852,7 @@
         <v>739</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>917</v>
+        <v>914</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -5859,7 +5880,7 @@
         <v>742</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -6153,7 +6174,7 @@
         <v>775</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -6223,7 +6244,7 @@
         <v>785</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -6545,7 +6566,7 @@
         <v>820</v>
       </c>
       <c r="D125" s="5" t="s">
-        <v>921</v>
+        <v>918</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -6615,7 +6636,7 @@
         <v>827</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>922</v>
+        <v>919</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -6629,7 +6650,7 @@
         <v>829</v>
       </c>
       <c r="D131" s="5" t="s">
-        <v>922</v>
+        <v>919</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -6671,7 +6692,7 @@
         <v>835</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -6685,7 +6706,7 @@
         <v>837</v>
       </c>
       <c r="D135" s="5" t="s">
-        <v>924</v>
+        <v>921</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -6699,7 +6720,7 @@
         <v>838</v>
       </c>
       <c r="D136" s="5" t="s">
-        <v>925</v>
+        <v>922</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -6713,7 +6734,7 @@
         <v>840</v>
       </c>
       <c r="D137" s="5" t="s">
-        <v>925</v>
+        <v>922</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -6755,7 +6776,7 @@
         <v>847</v>
       </c>
       <c r="D140" s="5" t="s">
-        <v>926</v>
+        <v>923</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -6797,7 +6818,7 @@
         <v>347</v>
       </c>
       <c r="D143" s="5" t="s">
-        <v>927</v>
+        <v>924</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -6811,7 +6832,7 @@
         <v>851</v>
       </c>
       <c r="D144" s="5" t="s">
-        <v>928</v>
+        <v>925</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -6867,7 +6888,7 @@
         <v>859</v>
       </c>
       <c r="D148" s="5" t="s">
-        <v>929</v>
+        <v>926</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -6881,7 +6902,7 @@
         <v>658</v>
       </c>
       <c r="D149" s="5" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -7007,7 +7028,7 @@
         <v>877</v>
       </c>
       <c r="D158" s="5" t="s">
-        <v>931</v>
+        <v>928</v>
       </c>
     </row>
     <row r="159" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -7021,7 +7042,7 @@
         <v>879</v>
       </c>
       <c r="D159" s="5" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
     </row>
     <row r="160" spans="1:4" ht="17" x14ac:dyDescent="0.25">
@@ -7029,10 +7050,10 @@
         <v>302</v>
       </c>
       <c r="B160" t="s">
-        <v>882</v>
-      </c>
-      <c r="C160" t="s">
         <v>881</v>
+      </c>
+      <c r="C160" s="6" t="s">
+        <v>938</v>
       </c>
       <c r="D160" s="5" t="s">
         <v>134</v>
@@ -7043,10 +7064,10 @@
         <v>303</v>
       </c>
       <c r="B161" t="s">
-        <v>883</v>
-      </c>
-      <c r="C161" t="s">
-        <v>884</v>
+        <v>882</v>
+      </c>
+      <c r="C161" s="6" t="s">
+        <v>939</v>
       </c>
       <c r="D161" s="5" t="s">
         <v>134</v>
@@ -7057,10 +7078,10 @@
         <v>304</v>
       </c>
       <c r="B162" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="C162" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="D162" s="5" t="s">
         <v>102</v>
@@ -7071,27 +7092,49 @@
         <v>305</v>
       </c>
       <c r="B163" t="s">
-        <v>888</v>
-      </c>
-      <c r="C163" t="s">
-        <v>887</v>
+        <v>885</v>
+      </c>
+      <c r="C163" s="6" t="s">
+        <v>940</v>
       </c>
       <c r="D163" s="5" t="s">
-        <v>933</v>
+        <v>930</v>
       </c>
     </row>
     <row r="164" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>934</v>
+        <v>931</v>
       </c>
       <c r="B164" t="s">
-        <v>935</v>
-      </c>
-      <c r="C164" t="s">
-        <v>936</v>
+        <v>932</v>
+      </c>
+      <c r="C164" s="6" t="s">
+        <v>937</v>
       </c>
       <c r="D164" s="5" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>941</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="C165" s="4" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>942</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>602</v>
       </c>
     </row>
   </sheetData>

</xml_diff>